<commit_message>
[#36] Adds support for crosssheet references
This allows you to have a range reference to a Cell on another sheet, that then points towards a cell on it's own sheet
</commit_message>
<xml_diff>
--- a/tests/resources/cross_sheet.xlsx
+++ b/tests/resources/cross_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\repos\xlcalculator\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC306D5-B736-46C6-86FD-E4F33A8113A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB520BE1-7D75-4658-9C1E-0FF044F6001B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="492" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="492" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
-    <t>Sheet2</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,23 +350,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
+      <c r="A2">
         <f>Sheet2!A2</f>
-        <v>Sheet2</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>Sheet2!A2+A1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3+Sheet2!A3</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -383,21 +388,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9386B469-6A5B-4C32-AEBA-B0257F4A4610}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
+      <c r="A1">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
+      <c r="A2">
         <f>A1</f>
-        <v>Sheet2</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actually evaluate open ended ranges.
</commit_message>
<xml_diff>
--- a/tests/resources/cross_sheet.xlsx
+++ b/tests/resources/cross_sheet.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="LastCell" vbProcedure="false">Sheet1!$C$4</definedName>
+    <definedName function="false" hidden="false" name="LastCell" vbProcedure="false">Sheet1!$C$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,6 +21,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Table</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,8 +111,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -116,64 +137,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">SUM(Sheet1!A:A)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <f aca="false">Sheet2!A2</f>
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">Sheet2!B2</f>
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">Sheet2!C2</f>
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <f aca="false">Sheet2!A2+A1</f>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <f aca="false">Sheet2!A2+A2</f>
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">Sheet2!B2+B1</f>
+      <c r="B4" s="1" t="n">
+        <f aca="false">Sheet2!B2+B2</f>
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">Sheet2!C2+C1</f>
+      <c r="C4" s="1" t="n">
+        <f aca="false">Sheet2!C2+C2</f>
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <f aca="false">A3+Sheet2!A3</f>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <f aca="false">A4+Sheet2!A3</f>
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">B3+Sheet2!B3</f>
+      <c r="B5" s="1" t="n">
+        <f aca="false">B4+Sheet2!B3</f>
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">C3+Sheet2!C3</f>
+      <c r="C5" s="1" t="n">
+        <f aca="false">C4+Sheet2!C3</f>
         <v>28</v>
       </c>
     </row>
@@ -195,47 +234,47 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <f aca="false">Sheet1!A4</f>
+      <c r="B1" s="1" t="n">
+        <f aca="false">Sheet1!A5</f>
         <v>4</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <f aca="false">Sheet1!B4</f>
+      <c r="C1" s="1" t="n">
+        <f aca="false">Sheet1!B5</f>
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <f aca="false">B1+1</f>
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">C1+1</f>
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">B2+1</f>
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">C2+1</f>
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Respond to comments. Increase coverage slightly.
</commit_message>
<xml_diff>
--- a/tests/resources/cross_sheet.xlsx
+++ b/tests/resources/cross_sheet.xlsx
@@ -137,10 +137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -155,7 +155,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -169,9 +169,12 @@
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <f aca="false">SUM(Sheet1!A:A)</f>
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,6 +189,10 @@
       <c r="C3" s="1" t="n">
         <f aca="false">Sheet2!C2</f>
         <v>13</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">SUM(2:2)</f>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -214,6 +221,11 @@
       <c r="C5" s="1" t="n">
         <f aca="false">C4+Sheet2!C3</f>
         <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>